<commit_message>
subject and mail body with variable values and minor errors solved
</commit_message>
<xml_diff>
--- a/Book11.xlsx
+++ b/Book11.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects July\Mail sender project\email_bold_done\email\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\F\Work\Parichaysharma\email_again_90%\email\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B92E178-E3EF-4457-87AF-356804E2C264}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4153D4D2-44C0-437A-9E4E-A59B62AB7997}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="13890" windowHeight="9360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,69 +22,27 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Email</t>
   </si>
   <si>
-    <t>asif</t>
-  </si>
-  <si>
-    <t>usman</t>
-  </si>
-  <si>
-    <t>mu.datascience219@gmail.com</t>
-  </si>
-  <si>
-    <t>junior python developer</t>
-  </si>
-  <si>
-    <t>zain</t>
-  </si>
-  <si>
-    <t>hr</t>
-  </si>
-  <si>
-    <t>zainjathol955@gmail.com</t>
-  </si>
-  <si>
-    <t>CEO123</t>
-  </si>
-  <si>
-    <t>asif5955iqbal@yahoo.com</t>
-  </si>
-  <si>
-    <t>aksah</t>
-  </si>
-  <si>
-    <t>abc</t>
-  </si>
-  <si>
-    <t>vinaysalva</t>
-  </si>
-  <si>
     <t>Sr. Developer</t>
   </si>
   <si>
     <t>savlavinay022@gmail.com</t>
   </si>
   <si>
-    <t>Name_is</t>
-  </si>
-  <si>
-    <t>Salry_is</t>
-  </si>
-  <si>
-    <t>Position_is</t>
-  </si>
-  <si>
-    <t>Akash Rasheed</t>
-  </si>
-  <si>
-    <t>python developer</t>
-  </si>
-  <si>
-    <t>akashanjum721@gmail.com</t>
+    <t>NAME</t>
+  </si>
+  <si>
+    <t>SALARY</t>
+  </si>
+  <si>
+    <t>POSITION</t>
+  </si>
+  <si>
+    <t>Vinay Savla</t>
   </si>
 </sst>
 </file>
@@ -482,126 +440,54 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18" customWidth="1"/>
-    <col min="2" max="2" width="17.6640625" customWidth="1"/>
+    <col min="2" max="2" width="17.7109375" customWidth="1"/>
     <col min="3" max="3" width="28" customWidth="1"/>
-    <col min="4" max="4" width="18.109375" customWidth="1"/>
+    <col min="4" max="4" width="18.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="B2">
-        <v>22222</v>
+        <v>24000</v>
       </c>
       <c r="C2" t="s">
-        <v>19</v>
+        <v>1</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
         <v>2</v>
-      </c>
-      <c r="B3">
-        <v>50000</v>
-      </c>
-      <c r="C3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4">
-        <v>15000</v>
-      </c>
-      <c r="C4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>1</v>
-      </c>
-      <c r="B5">
-        <v>100000</v>
-      </c>
-      <c r="C5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6">
-        <v>25000</v>
-      </c>
-      <c r="C6" t="s">
-        <v>11</v>
-      </c>
-      <c r="D6" s="2"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7">
-        <v>24000</v>
-      </c>
-      <c r="C7" t="s">
-        <v>13</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>14</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D5" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="D7" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="D2" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="D3" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="D4" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId6"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -611,7 +497,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -623,7 +509,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>